<commit_message>
added 7th week hw
</commit_message>
<xml_diff>
--- a/2.week/hw_2/Ornek.xlsx
+++ b/2.week/hw_2/Ornek.xlsx
@@ -7,15 +7,15 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="NewSheet" sheetId="3" r:id="rId3"/>
     <sheet name="Yenidosya" sheetId="4" r:id="rId4"/>
+    <sheet name="Yenidosya5" sheetId="5" r:id="rId5"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
-    <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
   <fonts count="1">
     <font>
@@ -46,9 +46,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -386,53 +385,53 @@
   </sheetViews>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="str">
+      <c r="A1" t="str">
         <v>ISIM</v>
       </c>
-      <c r="B1" s="1" t="str">
+      <c r="B1" t="str">
         <v>SOYISIM</v>
       </c>
-      <c r="C1" s="1" t="str">
+      <c r="C1" t="str">
         <v>YAS</v>
       </c>
-      <c r="D1" s="1" t="str">
+      <c r="D1" t="str">
         <v>ALDIGI MAAS</v>
       </c>
-      <c r="E1" s="1" t="str">
+      <c r="E1" t="str">
         <v>CINSIYETI</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="str">
+      <c r="A2" t="str">
         <v>Ali</v>
       </c>
-      <c r="B2" s="1" t="str">
+      <c r="B2" t="str">
         <v>Veli</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2">
         <v>33</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2">
         <v>7000</v>
       </c>
-      <c r="E2" s="1" t="str">
+      <c r="E2" t="str">
         <v>ERKEK</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="str">
+      <c r="A3" t="str">
         <v>Ayse</v>
       </c>
-      <c r="B3" s="1" t="str">
+      <c r="B3" t="str">
         <v>Fatma</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3">
         <v>45</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3">
         <v>6000</v>
       </c>
-      <c r="E3" s="1" t="str">
+      <c r="E3" t="str">
         <v>KADIN</v>
       </c>
     </row>
@@ -452,53 +451,53 @@
   </sheetViews>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="str">
+      <c r="A1" t="str">
         <v>ISIM</v>
       </c>
-      <c r="B1" s="1" t="str">
+      <c r="B1" t="str">
         <v>SOYISIM</v>
       </c>
-      <c r="C1" s="1" t="str">
+      <c r="C1" t="str">
         <v>YAS</v>
       </c>
-      <c r="D1" s="1" t="str">
+      <c r="D1" t="str">
         <v>ALDIGI MAAS</v>
       </c>
-      <c r="E1" s="1" t="str">
+      <c r="E1" t="str">
         <v>CINSIYETI</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="str">
+      <c r="A2" t="str">
         <v>Ahmet</v>
       </c>
-      <c r="B2" s="1" t="str">
+      <c r="B2" t="str">
         <v>Kaya</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2">
         <v>35</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2">
         <v>9000</v>
       </c>
-      <c r="E2" s="1" t="str">
+      <c r="E2" t="str">
         <v>ERKEK</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="str">
+      <c r="A3" t="str">
         <v>Müzeyyen</v>
       </c>
-      <c r="B3" s="1" t="str">
+      <c r="B3" t="str">
         <v>Senay</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3">
         <v>28</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3">
         <v>10000</v>
       </c>
-      <c r="E3" s="1" t="str">
+      <c r="E3" t="str">
         <v>KADIN</v>
       </c>
     </row>
@@ -518,142 +517,143 @@
   </sheetViews>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="str">
+      <c r="A1" t="str">
         <v>ISIM</v>
       </c>
-      <c r="B1" s="1" t="str">
+      <c r="B1" t="str">
         <v>SOYISIM</v>
       </c>
-      <c r="C1" s="1" t="str">
+      <c r="C1" t="str">
         <v>YAS</v>
       </c>
-      <c r="D1" s="1" t="str">
+      <c r="D1" t="str">
         <v>ALDIGI MAAS</v>
       </c>
-      <c r="E1" s="1" t="str">
+      <c r="E1" t="str">
         <v>CINSIYETI</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="str">
+      <c r="A2" t="str">
         <v>Cabbar</v>
       </c>
-      <c r="B2" s="1" t="str">
+      <c r="B2" t="str">
         <v>Mikail</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2">
         <v>22</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2">
         <v>6000</v>
       </c>
-      <c r="E2" s="1" t="str">
+      <c r="E2" t="str">
         <v>ERKEK</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="str">
+      <c r="A3" t="str">
         <v>Hans</v>
       </c>
-      <c r="B3" s="1" t="str">
+      <c r="B3" t="str">
         <v>Joe</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3">
         <v>39</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3">
         <v>16000</v>
       </c>
-      <c r="E3" s="1" t="str">
+      <c r="E3" t="str">
         <v>ERKEK</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="str">
+      <c r="A4" t="str">
         <v>Murtaza</v>
       </c>
-      <c r="B4" s="1" t="str">
+      <c r="B4" t="str">
         <v>Kaya</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4">
         <v>49</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4">
         <v>6000</v>
       </c>
-      <c r="E4" s="1" t="str">
+      <c r="E4" t="str">
         <v>ERKEK</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="str">
+      <c r="A5" t="str">
         <v>Marion</v>
       </c>
-      <c r="B5" s="1" t="str">
+      <c r="B5" t="str">
         <v>Minna</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5">
         <v>55</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5">
         <v>9000</v>
       </c>
-      <c r="E5" s="1" t="str">
+      <c r="E5" t="str">
         <v>KADIN</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="str">
+      <c r="A6" t="str">
         <v>Murat</v>
       </c>
-      <c r="B6" s="1" t="str">
+      <c r="B6" t="str">
         <v>Burhan</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6">
         <v>40</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6">
         <v>10000</v>
       </c>
-      <c r="E6" s="1" t="str">
+      <c r="E6" t="str">
         <v>ERKEK</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="str">
+      <c r="A7" t="str">
         <v>Abdurrezzak</v>
       </c>
-      <c r="B7" s="1" t="str">
+      <c r="B7" t="str">
         <v>Adigüzel</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7">
         <v>22</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7">
         <v>6000</v>
       </c>
-      <c r="E7" s="1" t="str">
+      <c r="E7" t="str">
         <v>ERKEK</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="str">
+      <c r="A8" t="str">
         <v>Mehmet</v>
       </c>
-      <c r="B8" s="1" t="str">
+      <c r="B8" t="str">
         <v>Sökmen</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8">
         <v>33</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8">
         <v>12000</v>
       </c>
-      <c r="E8" s="1" t="str">
+      <c r="E8" t="str">
         <v>ERKEK</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
     <ignoredError numberStoredAsText="1" sqref="A1:E8"/>
   </ignoredErrors>
@@ -668,138 +668,289 @@
   </sheetViews>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="str">
+      <c r="A1" t="str">
         <v>ISIM</v>
       </c>
-      <c r="B1" s="1" t="str">
+      <c r="B1" t="str">
         <v>SOYISIM</v>
       </c>
-      <c r="C1" s="1" t="str">
+      <c r="C1" t="str">
         <v>YAS</v>
       </c>
-      <c r="D1" s="1" t="str">
+      <c r="D1" t="str">
         <v>ALDIGI MAAS</v>
       </c>
-      <c r="E1" s="1" t="str">
+      <c r="E1" t="str">
         <v>CINSIYETI</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="str">
+      <c r="A2" t="str">
         <v>Cabbar</v>
       </c>
-      <c r="B2" s="1" t="str">
+      <c r="B2" t="str">
         <v>Mikail</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2">
         <v>22</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2">
         <v>6000</v>
       </c>
-      <c r="E2" s="1" t="str">
+      <c r="E2" t="str">
         <v>ERKEK</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="str">
+      <c r="A3" t="str">
         <v>Hans</v>
       </c>
-      <c r="B3" s="1" t="str">
+      <c r="B3" t="str">
         <v>Joe</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3">
         <v>39</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3">
         <v>16000</v>
       </c>
-      <c r="E3" s="1" t="str">
+      <c r="E3" t="str">
         <v>ERKEK</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="str">
+      <c r="A4" t="str">
         <v>Murtaza</v>
       </c>
-      <c r="B4" s="1" t="str">
+      <c r="B4" t="str">
         <v>Kaya</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4">
         <v>49</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4">
         <v>6000</v>
       </c>
-      <c r="E4" s="1" t="str">
+      <c r="E4" t="str">
         <v>ERKEK</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="str">
+      <c r="A5" t="str">
         <v>Marion</v>
       </c>
-      <c r="B5" s="1" t="str">
+      <c r="B5" t="str">
         <v>Minna</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5">
         <v>55</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5">
         <v>9000</v>
       </c>
-      <c r="E5" s="1" t="str">
+      <c r="E5" t="str">
         <v>KADIN</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="str">
+      <c r="A6" t="str">
         <v>Murat</v>
       </c>
-      <c r="B6" s="1" t="str">
+      <c r="B6" t="str">
         <v>Burhan</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6">
         <v>40</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6">
         <v>10000</v>
       </c>
-      <c r="E6" s="1" t="str">
+      <c r="E6" t="str">
         <v>ERKEK</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="str">
+      <c r="A7" t="str">
         <v>Abdurrezzak</v>
       </c>
-      <c r="B7" s="1" t="str">
+      <c r="B7" t="str">
         <v>Adigüzel</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7">
         <v>22</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7">
         <v>6000</v>
       </c>
-      <c r="E7" s="1" t="str">
+      <c r="E7" t="str">
         <v>ERKEK</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="str">
+      <c r="A8" t="str">
         <v>Mehmet</v>
       </c>
-      <c r="B8" s="1" t="str">
+      <c r="B8" t="str">
         <v>Sökmen</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8">
         <v>33</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8">
         <v>12000</v>
       </c>
-      <c r="E8" s="1" t="str">
+      <c r="E8" t="str">
+        <v>ERKEK</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:E8"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>ISIM</v>
+      </c>
+      <c r="B1" t="str">
+        <v>SOYISIM</v>
+      </c>
+      <c r="C1" t="str">
+        <v>YAS</v>
+      </c>
+      <c r="D1" t="str">
+        <v>ALDIGI MAAS</v>
+      </c>
+      <c r="E1" t="str">
+        <v>CINSIYETI</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>Cabbar</v>
+      </c>
+      <c r="B2" t="str">
+        <v>Mikail</v>
+      </c>
+      <c r="C2">
+        <v>22</v>
+      </c>
+      <c r="D2">
+        <v>6000</v>
+      </c>
+      <c r="E2" t="str">
+        <v>ERKEK</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>Hans</v>
+      </c>
+      <c r="B3" t="str">
+        <v>Joe</v>
+      </c>
+      <c r="C3">
+        <v>39</v>
+      </c>
+      <c r="D3">
+        <v>16000</v>
+      </c>
+      <c r="E3" t="str">
+        <v>ERKEK</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>Murtaza</v>
+      </c>
+      <c r="B4" t="str">
+        <v>Kaya</v>
+      </c>
+      <c r="C4">
+        <v>49</v>
+      </c>
+      <c r="D4">
+        <v>6000</v>
+      </c>
+      <c r="E4" t="str">
+        <v>ERKEK</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>Marion</v>
+      </c>
+      <c r="B5" t="str">
+        <v>Minna</v>
+      </c>
+      <c r="C5">
+        <v>55</v>
+      </c>
+      <c r="D5">
+        <v>9000</v>
+      </c>
+      <c r="E5" t="str">
+        <v>KADIN</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>Murat</v>
+      </c>
+      <c r="B6" t="str">
+        <v>Burhan</v>
+      </c>
+      <c r="C6">
+        <v>40</v>
+      </c>
+      <c r="D6">
+        <v>10000</v>
+      </c>
+      <c r="E6" t="str">
+        <v>ERKEK</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>Abdurrezzak</v>
+      </c>
+      <c r="B7" t="str">
+        <v>Adigüzel</v>
+      </c>
+      <c r="C7">
+        <v>22</v>
+      </c>
+      <c r="D7">
+        <v>6000</v>
+      </c>
+      <c r="E7" t="str">
+        <v>ERKEK</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>Mehmet</v>
+      </c>
+      <c r="B8" t="str">
+        <v>Sökmen</v>
+      </c>
+      <c r="C8">
+        <v>33</v>
+      </c>
+      <c r="D8">
+        <v>12000</v>
+      </c>
+      <c r="E8" t="str">
         <v>ERKEK</v>
       </c>
     </row>

</xml_diff>